<commit_message>
Updated curve fit method. Now robust even given negative values. Ready for Numerical Hessian.
</commit_message>
<xml_diff>
--- a/Evaluation result/TDM simulation/Predicted trip table 02_02.xlsx
+++ b/Evaluation result/TDM simulation/Predicted trip table 02_02.xlsx
@@ -514,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -556,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="Z2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA2" t="n">
         <v>0</v>
@@ -600,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -672,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="Z3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
         <v>0</v>
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -782,13 +782,13 @@
         <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4" t="n">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="AD4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE4" t="n">
         <v>0</v>
@@ -835,13 +835,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
         <v>0</v>
@@ -1014,13 +1014,13 @@
         <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
         <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" t="n">
         <v>0</v>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="AD6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6" t="n">
         <v>0</v>
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -1136,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
@@ -1267,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8" t="n">
         <v>0</v>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AA10" t="n">
         <v>0</v>
@@ -1585,10 +1585,10 @@
         <v>0</v>
       </c>
       <c r="U11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
         <v>0</v>
@@ -1609,10 +1609,10 @@
         <v>0</v>
       </c>
       <c r="AC11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="n">
         <v>0</v>
@@ -1647,13 +1647,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1662,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S12" t="n">
         <v>0</v>
@@ -1710,28 +1710,28 @@
         <v>0</v>
       </c>
       <c r="X12" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="n">
         <v>1</v>
       </c>
       <c r="Z12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AA12" t="n">
         <v>0</v>
       </c>
       <c r="AB12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC12" t="n">
         <v>0</v>
       </c>
       <c r="AD12" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AE12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF12" t="n">
         <v>0</v>
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -1811,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13" t="n">
         <v>0</v>
@@ -1820,31 +1820,31 @@
         <v>0</v>
       </c>
       <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD13" t="n">
         <v>2</v>
-      </c>
-      <c r="W13" t="n">
-        <v>0</v>
-      </c>
-      <c r="X13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>3</v>
       </c>
       <c r="AE13" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -1888,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" t="n">
         <v>0</v>
@@ -1912,7 +1912,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
         <v>0</v>
@@ -1933,10 +1933,10 @@
         <v>0</v>
       </c>
       <c r="U14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14" t="n">
         <v>0</v>
@@ -1948,19 +1948,19 @@
         <v>0</v>
       </c>
       <c r="Z14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA14" t="n">
         <v>0</v>
       </c>
       <c r="AB14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14" t="n">
         <v>0</v>
       </c>
       <c r="AD14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AE14" t="n">
         <v>0</v>
@@ -2022,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" t="n">
         <v>0</v>
@@ -2031,55 +2031,55 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="n">
         <v>3</v>
       </c>
-      <c r="P15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" t="n">
-        <v>0</v>
-      </c>
-      <c r="S15" t="n">
-        <v>0</v>
-      </c>
-      <c r="T15" t="n">
-        <v>0</v>
-      </c>
-      <c r="U15" t="n">
-        <v>0</v>
-      </c>
-      <c r="V15" t="n">
-        <v>0</v>
-      </c>
-      <c r="W15" t="n">
-        <v>0</v>
-      </c>
-      <c r="X15" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>0</v>
-      </c>
       <c r="AE15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15" t="n">
         <v>0</v>
@@ -2153,10 +2153,10 @@
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="Z16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA16" t="n">
         <v>0</v>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="AD16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE16" t="n">
         <v>0</v>
@@ -2272,7 +2272,7 @@
         <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
       <c r="Z17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17" t="n">
         <v>0</v>
@@ -2308,10 +2308,10 @@
         <v>0</v>
       </c>
       <c r="AD17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF17" t="n">
         <v>0</v>
@@ -2349,7 +2349,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -2370,7 +2370,7 @@
         <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
@@ -2379,13 +2379,13 @@
         <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" t="n">
         <v>1</v>
@@ -2397,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="U18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V18" t="n">
         <v>0</v>
@@ -2409,13 +2409,13 @@
         <v>0</v>
       </c>
       <c r="Y18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z18" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="AA18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB18" t="n">
         <v>0</v>
@@ -2486,7 +2486,7 @@
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
         <v>0</v>
@@ -2507,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
@@ -2528,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="Z19" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AA19" t="n">
         <v>0</v>
@@ -2540,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="AD19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE19" t="n">
         <v>0</v>
@@ -2629,7 +2629,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V20" t="n">
         <v>0</v>
@@ -2638,13 +2638,13 @@
         <v>0</v>
       </c>
       <c r="X20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y20" t="n">
         <v>0</v>
       </c>
       <c r="Z20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA20" t="n">
         <v>0</v>
@@ -2656,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="AD20" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AE20" t="n">
         <v>0</v>
@@ -2721,10 +2721,10 @@
         <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
@@ -2742,37 +2742,37 @@
         <v>0</v>
       </c>
       <c r="T21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U21" t="n">
         <v>1</v>
       </c>
       <c r="V21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD21" t="n">
         <v>7</v>
-      </c>
-      <c r="W21" t="n">
-        <v>0</v>
-      </c>
-      <c r="X21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>10</v>
-      </c>
-      <c r="AA21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD21" t="n">
-        <v>8</v>
       </c>
       <c r="AE21" t="n">
         <v>0</v>
@@ -2831,16 +2831,16 @@
         <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" t="n">
         <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O22" t="n">
         <v>0</v>
@@ -2858,16 +2858,16 @@
         <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V22" t="n">
         <v>3</v>
       </c>
       <c r="W22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22" t="n">
         <v>0</v>
@@ -2876,19 +2876,19 @@
         <v>0</v>
       </c>
       <c r="Z22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD22" t="n">
         <v>2</v>
-      </c>
-      <c r="AA22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>12</v>
       </c>
       <c r="AE22" t="n">
         <v>0</v>
@@ -2977,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="U23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V23" t="n">
         <v>0</v>
@@ -2986,13 +2986,13 @@
         <v>0</v>
       </c>
       <c r="X23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23" t="n">
         <v>0</v>
       </c>
       <c r="Z23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA23" t="n">
         <v>0</v>
@@ -3004,7 +3004,7 @@
         <v>0</v>
       </c>
       <c r="AD23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE23" t="n">
         <v>0</v>
@@ -3039,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
         <v>1</v>
@@ -3066,16 +3066,16 @@
         <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P24" t="n">
         <v>0</v>
@@ -3090,28 +3090,28 @@
         <v>0</v>
       </c>
       <c r="T24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U24" t="n">
         <v>0</v>
       </c>
       <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="n">
         <v>2</v>
       </c>
-      <c r="W24" t="n">
-        <v>0</v>
-      </c>
       <c r="X24" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Y24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA24" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AB24" t="n">
         <v>0</v>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="AD24" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="AE24" t="n">
         <v>1</v>
@@ -3152,109 +3152,109 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
+        <v>12</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>4</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>26</v>
+      </c>
+      <c r="L25" t="n">
+        <v>20</v>
+      </c>
+      <c r="M25" t="n">
+        <v>22</v>
+      </c>
+      <c r="N25" t="n">
+        <v>21</v>
+      </c>
+      <c r="O25" t="n">
+        <v>13</v>
+      </c>
+      <c r="P25" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>18</v>
+      </c>
+      <c r="R25" t="n">
+        <v>36</v>
+      </c>
+      <c r="S25" t="n">
+        <v>14</v>
+      </c>
+      <c r="T25" t="n">
+        <v>22</v>
+      </c>
+      <c r="U25" t="n">
+        <v>18</v>
+      </c>
+      <c r="V25" t="n">
+        <v>21</v>
+      </c>
+      <c r="W25" t="n">
+        <v>11</v>
+      </c>
+      <c r="X25" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y25" t="n">
         <v>7</v>
       </c>
-      <c r="E25" t="n">
-        <v>7</v>
-      </c>
-      <c r="F25" t="n">
+      <c r="Z25" t="n">
+        <v>264</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>255</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>15</v>
+      </c>
+      <c r="AI25" t="n">
         <v>5</v>
       </c>
-      <c r="G25" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>6</v>
-      </c>
-      <c r="K25" t="n">
-        <v>3</v>
-      </c>
-      <c r="L25" t="n">
-        <v>12</v>
-      </c>
-      <c r="M25" t="n">
-        <v>5</v>
-      </c>
-      <c r="N25" t="n">
-        <v>7</v>
-      </c>
-      <c r="O25" t="n">
-        <v>4</v>
-      </c>
-      <c r="P25" t="n">
-        <v>9</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>22</v>
-      </c>
-      <c r="R25" t="n">
-        <v>30</v>
-      </c>
-      <c r="S25" t="n">
-        <v>10</v>
-      </c>
-      <c r="T25" t="n">
-        <v>7</v>
-      </c>
-      <c r="U25" t="n">
-        <v>5</v>
-      </c>
-      <c r="V25" t="n">
-        <v>7</v>
-      </c>
-      <c r="W25" t="n">
-        <v>1</v>
-      </c>
-      <c r="X25" t="n">
-        <v>7</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>11</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>796</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB25" t="n">
-        <v>15</v>
-      </c>
-      <c r="AC25" t="n">
-        <v>7</v>
-      </c>
-      <c r="AD25" t="n">
-        <v>140</v>
-      </c>
-      <c r="AE25" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF25" t="n">
-        <v>8</v>
-      </c>
-      <c r="AG25" t="n">
-        <v>4</v>
-      </c>
-      <c r="AH25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI25" t="n">
-        <v>1</v>
-      </c>
       <c r="AJ25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK25" t="n">
         <v>0</v>
@@ -3268,95 +3268,95 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>1</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="n">
         <v>2</v>
       </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="n">
-        <v>1</v>
-      </c>
-      <c r="K26" t="n">
-        <v>5</v>
-      </c>
-      <c r="L26" t="n">
+      <c r="V26" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z26" t="n">
         <v>14</v>
       </c>
-      <c r="M26" t="n">
-        <v>7</v>
-      </c>
-      <c r="N26" t="n">
-        <v>7</v>
-      </c>
-      <c r="O26" t="n">
-        <v>6</v>
-      </c>
-      <c r="P26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>7</v>
-      </c>
-      <c r="R26" t="n">
-        <v>4</v>
-      </c>
-      <c r="S26" t="n">
+      <c r="AA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>42</v>
+      </c>
+      <c r="AE26" t="n">
         <v>2</v>
       </c>
-      <c r="T26" t="n">
-        <v>5</v>
-      </c>
-      <c r="U26" t="n">
-        <v>21</v>
-      </c>
-      <c r="V26" t="n">
-        <v>6</v>
-      </c>
-      <c r="W26" t="n">
-        <v>1</v>
-      </c>
-      <c r="X26" t="n">
-        <v>5</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>31</v>
-      </c>
-      <c r="Z26" t="n">
-        <v>15</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB26" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC26" t="n">
-        <v>39</v>
-      </c>
-      <c r="AD26" t="n">
-        <v>508</v>
-      </c>
-      <c r="AE26" t="n">
-        <v>1</v>
-      </c>
       <c r="AF26" t="n">
         <v>0</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>0</v>
       </c>
       <c r="AI26" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AJ26" t="n">
         <v>0</v>
@@ -3471,7 +3471,7 @@
         <v>1</v>
       </c>
       <c r="AE27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF27" t="n">
         <v>0</v>
@@ -3572,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="Z28" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AA28" t="n">
         <v>0</v>
@@ -3581,10 +3581,10 @@
         <v>2</v>
       </c>
       <c r="AC28" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AD28" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE28" t="n">
         <v>0</v>
@@ -3599,7 +3599,7 @@
         <v>0</v>
       </c>
       <c r="AI28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ28" t="n">
         <v>0</v>
@@ -3667,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="S29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T29" t="n">
         <v>0</v>
@@ -3688,25 +3688,25 @@
         <v>0</v>
       </c>
       <c r="Z29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA29" t="n">
         <v>0</v>
       </c>
       <c r="AB29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC29" t="n">
         <v>0</v>
       </c>
       <c r="AD29" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="AE29" t="n">
         <v>0</v>
       </c>
       <c r="AF29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG29" t="n">
         <v>0</v>
@@ -3732,7 +3732,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -3741,7 +3741,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -3780,64 +3780,64 @@
         <v>0</v>
       </c>
       <c r="R30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S30" t="n">
         <v>0</v>
       </c>
       <c r="T30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U30" t="n">
         <v>1</v>
       </c>
       <c r="V30" t="n">
+        <v>1</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
         <v>3</v>
       </c>
-      <c r="W30" t="n">
-        <v>1</v>
-      </c>
-      <c r="X30" t="n">
-        <v>0</v>
-      </c>
       <c r="Y30" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Z30" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="AA30" t="n">
         <v>0</v>
       </c>
       <c r="AB30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD30" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AE30" t="n">
         <v>0</v>
       </c>
       <c r="AF30" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG30" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AH30" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AI30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ30" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="AK30" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AL30" t="n">
         <v>0</v>
@@ -3914,13 +3914,13 @@
         <v>0</v>
       </c>
       <c r="X31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y31" t="n">
         <v>1</v>
       </c>
       <c r="Z31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA31" t="n">
         <v>0</v>
@@ -3935,7 +3935,7 @@
         <v>0</v>
       </c>
       <c r="AE31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF31" t="n">
         <v>0</v>
@@ -4012,7 +4012,7 @@
         <v>0</v>
       </c>
       <c r="R32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -4036,7 +4036,7 @@
         <v>0</v>
       </c>
       <c r="Z32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA32" t="n">
         <v>0</v>
@@ -4045,10 +4045,10 @@
         <v>0</v>
       </c>
       <c r="AC32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AD32" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AE32" t="n">
         <v>0</v>
@@ -4060,13 +4060,13 @@
         <v>0</v>
       </c>
       <c r="AH32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI32" t="n">
         <v>0</v>
       </c>
       <c r="AJ32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK32" t="n">
         <v>0</v>
@@ -4164,7 +4164,7 @@
         <v>0</v>
       </c>
       <c r="AD33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE33" t="n">
         <v>0</v>
@@ -4173,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="AG33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH33" t="n">
         <v>0</v>
@@ -4182,7 +4182,7 @@
         <v>0</v>
       </c>
       <c r="AJ33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK33" t="n">
         <v>0</v>
@@ -4277,13 +4277,13 @@
         <v>0</v>
       </c>
       <c r="AC34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF34" t="n">
         <v>0</v>
@@ -4298,10 +4298,10 @@
         <v>0</v>
       </c>
       <c r="AJ34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL34" t="n">
         <v>0</v>
@@ -4384,7 +4384,7 @@
         <v>0</v>
       </c>
       <c r="Z35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA35" t="n">
         <v>0</v>
@@ -4393,13 +4393,13 @@
         <v>0</v>
       </c>
       <c r="AC35" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD35" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AE35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF35" t="n">
         <v>0</v>
@@ -4509,10 +4509,10 @@
         <v>0</v>
       </c>
       <c r="AC36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE36" t="n">
         <v>0</v>
@@ -4589,7 +4589,7 @@
         <v>0</v>
       </c>
       <c r="Q37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R37" t="n">
         <v>0</v>
@@ -4628,7 +4628,7 @@
         <v>0</v>
       </c>
       <c r="AD37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE37" t="n">
         <v>0</v>

</xml_diff>